<commit_message>
Segunda modificacion de Libro1 para subir a nube
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOMERC LAP\Documents\Hortencia\Tec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOMERC LAP\Documents\Hortencia\Tec\appMovil\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Hola hoja de excel de Hortencia Castro</t>
+  </si>
+  <si>
+    <t>Segunda modificacion para fines practicos. 10/19/18 8:05</t>
   </si>
 </sst>
 </file>
@@ -345,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,6 +366,11 @@
         <v>43392</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>